<commit_message>
Fixed timetable rendering in react; Linter warns instead of errors for unused imports and variables; Renamed SlotDataClass to SlotDataClasses
</commit_message>
<xml_diff>
--- a/SAMPLE_DATA/xlsx/subject_and_teacher_cs.xlsx
+++ b/SAMPLE_DATA/xlsx/subject_and_teacher_cs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pranav\Timetable_Manager_Backend\src\sampleData\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pranav\Restructured Timetable\timetable-manager-backend\SAMPLE_DATA\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D0411F-7E33-45AB-8BCE-B184522BEABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95585CC-210E-43D6-A96E-67822F70D99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -719,12 +719,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1206,7 +1205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
@@ -3265,11 +3264,11 @@
       <c r="F76" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G76" s="4">
+      <c r="G76">
         <f t="shared" ref="G76" si="2">IF(ISNUMBER(SEARCH("Lab", C76)), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="H76" s="4">
+      <c r="H76">
         <v>1</v>
       </c>
     </row>

</xml_diff>